<commit_message>
Changing Color scale for Figure 3
</commit_message>
<xml_diff>
--- a/06_USMA_ExpEvol_Data/F05_ExpEvol_Resistance_Chr9_Data/UMAG_11067_qPCR.xlsx
+++ b/06_USMA_ExpEvol_Data/F05_ExpEvol_Resistance_Chr9_Data/UMAG_11067_qPCR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SilverStone\Documents\PaperToMBE\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SilverStone\Documents\PaperToMBE\GitLab_Repository\06_USMA_ExpEvol_Data\F05_ExpEvol_Resistance_Chr9_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73066AB2-F314-42CF-9365-A8D46149BF90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3A612F-2A83-43FE-B603-2F9537B7796F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{06FAAF3D-9828-4322-93D7-7CC4AAE6A5C9}"/>
   </bookViews>
@@ -295,12 +295,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -308,6 +302,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -340,8 +340,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>152475</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 13">
@@ -623,7 +623,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 13">
@@ -1643,7 +1643,7 @@
   <dimension ref="B1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1657,7 +1657,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21">
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1720,46 +1720,46 @@
       <c r="K7" s="9"/>
     </row>
     <row r="8" spans="2:21">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="16" t="s">
+      <c r="H8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="I8" s="16" t="s">
+      <c r="I8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="J8" s="7"/>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-      <c r="O8" s="11" t="s">
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="O8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="S8" s="11" t="s">
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="S8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="16"/>
     </row>
     <row r="9" spans="2:21">
       <c r="B9" s="4" t="s">
@@ -1786,7 +1786,7 @@
       <c r="I9" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="12"/>
+      <c r="K9" s="10"/>
     </row>
     <row r="10" spans="2:21">
       <c r="B10" t="s">
@@ -1813,16 +1813,16 @@
       <c r="I10" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="10">
         <f>(F9-F10)</f>
         <v>0.45835304260253906</v>
       </c>
-      <c r="L10" s="12">
-        <f t="shared" ref="L10:M10" si="0">(G9-G10)</f>
+      <c r="L10" s="10">
+        <f>(G9-G10)</f>
         <v>1.6613445281982422</v>
       </c>
-      <c r="M10" s="12">
-        <f t="shared" si="0"/>
+      <c r="M10" s="10">
+        <f t="shared" ref="L10:M10" si="0">(H9-H10)</f>
         <v>1.786407470703125</v>
       </c>
       <c r="O10" s="1">
@@ -1875,16 +1875,16 @@
       <c r="I11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="10">
         <f>(F9-F11)</f>
         <v>0.18293571472167969</v>
       </c>
-      <c r="L11" s="12">
-        <f t="shared" ref="L11:M11" si="3">(G9-G11)</f>
+      <c r="L11" s="10">
+        <f>(G9-G11)</f>
         <v>1.1361770629882813</v>
       </c>
-      <c r="M11" s="12">
-        <f t="shared" si="3"/>
+      <c r="M11" s="10">
+        <f t="shared" ref="L11:M11" si="3">(H9-H11)</f>
         <v>1.4855937957763672</v>
       </c>
       <c r="O11" s="1">
@@ -1963,15 +1963,15 @@
       <c r="I13" t="s">
         <v>27</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="10">
         <f>F12-F13</f>
         <v>1.2969112396240234</v>
       </c>
-      <c r="L13" s="12">
+      <c r="L13" s="10">
         <f>G12-G13</f>
         <v>2.8573627471923828</v>
       </c>
-      <c r="M13" s="12">
+      <c r="M13" s="10">
         <f>H12-H13</f>
         <v>2.6482505798339844</v>
       </c>
@@ -2014,28 +2014,28 @@
         <v>27</v>
       </c>
       <c r="J14" s="7"/>
-      <c r="K14" s="13">
+      <c r="K14" s="11">
         <f>F12-F14</f>
         <v>1.4383926391601563</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="11">
         <f>G12-G14</f>
         <v>3.1799583435058594</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="11">
         <f>H12-H14</f>
         <v>2.4190387725830078</v>
       </c>
       <c r="N14" s="7"/>
-      <c r="O14" s="14">
+      <c r="O14" s="12">
         <f>($L$3)^(K14)</f>
         <v>2.9271534950456832</v>
       </c>
-      <c r="P14" s="14">
+      <c r="P14" s="12">
         <f t="shared" si="5"/>
         <v>10.744957433929892</v>
       </c>
-      <c r="Q14" s="14">
+      <c r="Q14" s="12">
         <f t="shared" si="5"/>
         <v>6.0876802388426743</v>
       </c>
@@ -2095,15 +2095,15 @@
       <c r="I16" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="10">
         <f>F15-F16</f>
         <v>4.6744651794433594</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="10">
         <f t="shared" ref="L16:M16" si="6">G15-G16</f>
         <v>4.1472949981689453</v>
       </c>
-      <c r="M16" s="12">
+      <c r="M16" s="10">
         <f t="shared" si="6"/>
         <v>4.9837837219238281</v>
       </c>
@@ -2157,15 +2157,15 @@
       <c r="I17" t="s">
         <v>27</v>
       </c>
-      <c r="K17" s="12">
+      <c r="K17" s="10">
         <f>F15-F17</f>
         <v>6.657470703125</v>
       </c>
-      <c r="L17" s="12">
+      <c r="L17" s="10">
         <f t="shared" ref="L17:M17" si="9">G15-G17</f>
         <v>5.898500442504897</v>
       </c>
-      <c r="M17" s="12">
+      <c r="M17" s="10">
         <f t="shared" si="9"/>
         <v>6.9003028869629865</v>
       </c>
@@ -2245,15 +2245,15 @@
       <c r="I19" t="s">
         <v>27</v>
       </c>
-      <c r="K19" s="12">
+      <c r="K19" s="10">
         <f>F18-F19</f>
         <v>4.180999755859375</v>
       </c>
-      <c r="L19" s="12">
+      <c r="L19" s="10">
         <f t="shared" ref="L19:M19" si="10">G18-G19</f>
         <v>3.7310447692871094</v>
       </c>
-      <c r="M19" s="12">
+      <c r="M19" s="10">
         <f t="shared" si="10"/>
         <v>4.315521240234375</v>
       </c>
@@ -2296,28 +2296,28 @@
         <v>27</v>
       </c>
       <c r="J20" s="7"/>
-      <c r="K20" s="13">
+      <c r="K20" s="11">
         <f>F18-F20</f>
         <v>5.4270191192626953</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="11">
         <f t="shared" ref="L20:M20" si="12">G18-G20</f>
         <v>5.2431182861328125</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="11">
         <f t="shared" si="12"/>
         <v>5.3381710052490234</v>
       </c>
       <c r="N20" s="7"/>
-      <c r="O20" s="14">
+      <c r="O20" s="12">
         <f>($L$3)^(K20)</f>
         <v>57.529034439831648</v>
       </c>
-      <c r="P20" s="14">
+      <c r="P20" s="12">
         <f t="shared" si="11"/>
         <v>50.147729114043457</v>
       </c>
-      <c r="Q20" s="14">
+      <c r="Q20" s="12">
         <f>($L$3)^(M20)</f>
         <v>53.836299483919262</v>
       </c>
@@ -2377,15 +2377,15 @@
       <c r="I22" t="s">
         <v>27</v>
       </c>
-      <c r="K22" s="12">
+      <c r="K22" s="10">
         <f>F21-F22</f>
         <v>8.0286865234375</v>
       </c>
-      <c r="L22" s="12">
+      <c r="L22" s="10">
         <f t="shared" ref="L22:M22" si="13">G21-G22</f>
         <v>8.3727569580078125</v>
       </c>
-      <c r="M22" s="12">
+      <c r="M22" s="10">
         <f t="shared" si="13"/>
         <v>7.3423919677734375</v>
       </c>
@@ -2439,15 +2439,15 @@
       <c r="I23" t="s">
         <v>27</v>
       </c>
-      <c r="K23" s="12">
+      <c r="K23" s="10">
         <f>F21-F23</f>
         <v>10.20759391784668</v>
       </c>
-      <c r="L23" s="12">
+      <c r="L23" s="10">
         <f>G21-G23</f>
         <v>10.188282012939503</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="10">
         <f t="shared" ref="M23" si="16">H21-H23</f>
         <v>9.9123439788818359</v>
       </c>
@@ -2527,15 +2527,15 @@
       <c r="I25" t="s">
         <v>27</v>
       </c>
-      <c r="K25" s="12">
+      <c r="K25" s="10">
         <f>F24-F25</f>
         <v>7.1657962799072266</v>
       </c>
-      <c r="L25" s="12">
+      <c r="L25" s="10">
         <f t="shared" ref="L25:M25" si="17">G24-G25</f>
         <v>8.4934787750244141</v>
       </c>
-      <c r="M25" s="12">
+      <c r="M25" s="10">
         <f t="shared" si="17"/>
         <v>6.6514415740966903</v>
       </c>
@@ -2578,28 +2578,28 @@
         <v>27</v>
       </c>
       <c r="J26" s="7"/>
-      <c r="K26" s="13">
+      <c r="K26" s="11">
         <f>F24-F26</f>
         <v>7.0511074066162109</v>
       </c>
-      <c r="L26" s="13">
+      <c r="L26" s="11">
         <f t="shared" ref="L26:M26" si="19">G24-G26</f>
         <v>7.3788509368896484</v>
       </c>
-      <c r="M26" s="13">
+      <c r="M26" s="11">
         <f t="shared" si="19"/>
         <v>7.2458953857421911</v>
       </c>
       <c r="N26" s="7"/>
-      <c r="O26" s="14">
+      <c r="O26" s="12">
         <f>($L$3)^(K26)</f>
         <v>193.44184351075484</v>
       </c>
-      <c r="P26" s="14">
+      <c r="P26" s="12">
         <f>($L$3)^(L26)</f>
         <v>247.07676081680168</v>
       </c>
-      <c r="Q26" s="14">
+      <c r="Q26" s="12">
         <f>($L$3)^(M26)</f>
         <v>223.72614865710224</v>
       </c>

</xml_diff>